<commit_message>
Code refactors and ground truth file update
- Pulling from main branch of unlogged-spring-maven-demo.
- Moving utils and entities out of tests.
- Updating ground truth file, correcting spelling errors for cases of SIMILAR.
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-ground-truth-integration-mode.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-ground-truth-integration-mode.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3321" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3321" uniqueCount="524">
   <si>
     <t>Class</t>
   </si>
@@ -1295,9 +1295,6 @@
   <si>
     <t>save
 (Lorg/unlogged/demo/models/CustomerProfileRequest;)Lorg/unlogged/demo/models/CustomerProfile;</t>
-  </si>
-  <si>
-    <t>SIMIALR</t>
   </si>
   <si>
     <t>{"customerid":2,"customername":"string","dateofbirth":"string","email":"string","contactnumber":"string","address":"string","referralcodes":["string"]}</t>
@@ -8451,10 +8448,10 @@
         <v>291</v>
       </c>
       <c r="F215" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G215" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G215" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>15</v>
@@ -8468,7 +8465,7 @@
         <v>346</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>346</v>
@@ -8483,7 +8480,7 @@
         <v>51</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H216" s="1" t="s">
         <v>15</v>
@@ -8497,7 +8494,7 @@
         <v>346</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>346</v>
@@ -8512,7 +8509,7 @@
         <v>51</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H217" s="1" t="s">
         <v>15</v>
@@ -8526,7 +8523,7 @@
         <v>346</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>346</v>
@@ -8541,7 +8538,7 @@
         <v>51</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>15</v>
@@ -8555,7 +8552,7 @@
         <v>346</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>346</v>
@@ -8570,7 +8567,7 @@
         <v>51</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H219" s="1" t="s">
         <v>15</v>
@@ -8584,7 +8581,7 @@
         <v>346</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>346</v>
@@ -8599,10 +8596,10 @@
         <v>13</v>
       </c>
       <c r="G220" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H220" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>39</v>
@@ -8610,13 +8607,13 @@
     </row>
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B221" s="1" t="s">
-        <v>363</v>
-      </c>
       <c r="C221" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>11</v>
@@ -8639,19 +8636,19 @@
     </row>
     <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E222" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="F222" s="2" t="s">
         <v>13</v>
@@ -8668,13 +8665,13 @@
     </row>
     <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>11</v>
@@ -8697,19 +8694,19 @@
     </row>
     <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F224" s="2" t="s">
         <v>13</v>
@@ -8726,13 +8723,13 @@
     </row>
     <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>11</v>
@@ -8755,13 +8752,13 @@
     </row>
     <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>11</v>
@@ -8784,25 +8781,25 @@
     </row>
     <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B227" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G227" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F227" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G227" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="H227" s="1" t="s">
         <v>15</v>
@@ -8813,19 +8810,19 @@
     </row>
     <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E228" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="F228" s="2" t="s">
         <v>13</v>
@@ -8842,13 +8839,13 @@
     </row>
     <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>11</v>
@@ -8871,19 +8868,19 @@
     </row>
     <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F230" s="2" t="s">
         <v>13</v>
@@ -8900,13 +8897,13 @@
     </row>
     <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>11</v>
@@ -8929,19 +8926,19 @@
     </row>
     <row r="232" ht="15.75" customHeight="1">
       <c r="A232" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F232" s="2" t="s">
         <v>13</v>
@@ -8958,13 +8955,13 @@
     </row>
     <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>11</v>
@@ -8987,13 +8984,13 @@
     </row>
     <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>11</v>
@@ -9016,13 +9013,13 @@
     </row>
     <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D235" s="1" t="s">
         <v>11</v>
@@ -9045,13 +9042,13 @@
     </row>
     <row r="236" ht="15.75" customHeight="1">
       <c r="A236" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>11</v>
@@ -9074,13 +9071,13 @@
     </row>
     <row r="237" ht="15.75" customHeight="1">
       <c r="A237" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>11</v>
@@ -9103,19 +9100,19 @@
     </row>
     <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F238" s="4" t="s">
         <v>13</v>
@@ -9132,13 +9129,13 @@
     </row>
     <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>11</v>
@@ -9161,19 +9158,19 @@
     </row>
     <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F240" s="4" t="s">
         <v>13</v>
@@ -9190,13 +9187,13 @@
     </row>
     <row r="241" ht="15.75" customHeight="1">
       <c r="A241" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>11</v>
@@ -9219,19 +9216,19 @@
     </row>
     <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F242" s="4" t="s">
         <v>13</v>
@@ -9248,13 +9245,13 @@
     </row>
     <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>11</v>
@@ -9277,19 +9274,19 @@
     </row>
     <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F244" s="4" t="s">
         <v>13</v>
@@ -9306,13 +9303,13 @@
     </row>
     <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>11</v>
@@ -9335,13 +9332,13 @@
     </row>
     <row r="246" ht="15.75" customHeight="1">
       <c r="A246" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>11</v>
@@ -9364,13 +9361,13 @@
     </row>
     <row r="247" ht="15.75" customHeight="1">
       <c r="A247" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>11</v>
@@ -9393,13 +9390,13 @@
     </row>
     <row r="248" ht="15.75" customHeight="1">
       <c r="A248" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>11</v>
@@ -9422,13 +9419,13 @@
     </row>
     <row r="249" ht="15.75" customHeight="1">
       <c r="A249" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>11</v>
@@ -9451,19 +9448,19 @@
     </row>
     <row r="250" ht="15.75" customHeight="1">
       <c r="A250" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F250" s="4" t="s">
         <v>13</v>
@@ -9480,13 +9477,13 @@
     </row>
     <row r="251" ht="15.75" customHeight="1">
       <c r="A251" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>11</v>
@@ -9509,19 +9506,19 @@
     </row>
     <row r="252" ht="15.75" customHeight="1">
       <c r="A252" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F252" s="4" t="s">
         <v>13</v>
@@ -9538,13 +9535,13 @@
     </row>
     <row r="253" ht="15.75" customHeight="1">
       <c r="A253" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>11</v>
@@ -9567,19 +9564,19 @@
     </row>
     <row r="254" ht="15.75" customHeight="1">
       <c r="A254" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F254" s="4" t="s">
         <v>13</v>
@@ -9596,13 +9593,13 @@
     </row>
     <row r="255" ht="15.75" customHeight="1">
       <c r="A255" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>11</v>
@@ -9625,19 +9622,19 @@
     </row>
     <row r="256" ht="15.75" customHeight="1">
       <c r="A256" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F256" s="4" t="s">
         <v>13</v>
@@ -9654,13 +9651,13 @@
     </row>
     <row r="257" ht="15.75" customHeight="1">
       <c r="A257" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>11</v>
@@ -9683,19 +9680,19 @@
     </row>
     <row r="258" ht="15.75" customHeight="1">
       <c r="A258" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F258" s="4" t="s">
         <v>13</v>
@@ -9712,13 +9709,13 @@
     </row>
     <row r="259" ht="15.75" customHeight="1">
       <c r="A259" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D259" s="1" t="s">
         <v>11</v>
@@ -9741,19 +9738,19 @@
     </row>
     <row r="260" ht="15.75" customHeight="1">
       <c r="A260" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D260" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F260" s="4" t="s">
         <v>13</v>
@@ -9770,13 +9767,13 @@
     </row>
     <row r="261" ht="15.75" customHeight="1">
       <c r="A261" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>11</v>
@@ -9799,19 +9796,19 @@
     </row>
     <row r="262" ht="15.75" customHeight="1">
       <c r="A262" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D262" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F262" s="4" t="s">
         <v>13</v>
@@ -9828,13 +9825,13 @@
     </row>
     <row r="263" ht="15.75" customHeight="1">
       <c r="A263" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>11</v>
@@ -9846,7 +9843,7 @@
         <v>51</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H263" s="1" t="s">
         <v>15</v>
@@ -9857,13 +9854,13 @@
     </row>
     <row r="264" ht="15.75" customHeight="1">
       <c r="A264" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B264" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B264" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="C264" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>11</v>
@@ -9886,13 +9883,13 @@
     </row>
     <row r="265" ht="15.75" customHeight="1">
       <c r="A265" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>11</v>
@@ -9915,13 +9912,13 @@
     </row>
     <row r="266" ht="15.75" customHeight="1">
       <c r="A266" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>11</v>
@@ -9944,13 +9941,13 @@
     </row>
     <row r="267" ht="15.75" customHeight="1">
       <c r="A267" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>11</v>
@@ -9973,13 +9970,13 @@
     </row>
     <row r="268" ht="15.75" customHeight="1">
       <c r="A268" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D268" s="1" t="s">
         <v>11</v>
@@ -10002,13 +9999,13 @@
     </row>
     <row r="269" ht="15.75" customHeight="1">
       <c r="A269" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>11</v>
@@ -10031,13 +10028,13 @@
     </row>
     <row r="270" ht="15.75" customHeight="1">
       <c r="A270" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D270" s="1" t="s">
         <v>11</v>
@@ -10049,7 +10046,7 @@
         <v>13</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H270" s="1" t="s">
         <v>15</v>
@@ -10060,13 +10057,13 @@
     </row>
     <row r="271" ht="15.75" customHeight="1">
       <c r="A271" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>35</v>
@@ -10078,10 +10075,10 @@
         <v>20</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H271" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I271" s="1" t="s">
         <v>39</v>
@@ -10089,13 +10086,13 @@
     </row>
     <row r="272" ht="15.75" customHeight="1">
       <c r="A272" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D272" s="1" t="s">
         <v>35</v>
@@ -10107,10 +10104,10 @@
         <v>20</v>
       </c>
       <c r="G272" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H272" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I272" s="1" t="s">
         <v>39</v>
@@ -10118,13 +10115,13 @@
     </row>
     <row r="273" ht="15.75" customHeight="1">
       <c r="A273" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>35</v>
@@ -10136,10 +10133,10 @@
         <v>20</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H273" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I273" s="1" t="s">
         <v>39</v>
@@ -10147,13 +10144,13 @@
     </row>
     <row r="274" ht="15.75" customHeight="1">
       <c r="A274" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>35</v>
@@ -10176,13 +10173,13 @@
     </row>
     <row r="275" ht="15.75" customHeight="1">
       <c r="A275" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>35</v>
@@ -10194,10 +10191,10 @@
         <v>20</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H275" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I275" s="1" t="s">
         <v>39</v>
@@ -10205,13 +10202,13 @@
     </row>
     <row r="276" ht="15.75" customHeight="1">
       <c r="A276" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>35</v>
@@ -10223,10 +10220,10 @@
         <v>20</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H276" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I276" s="1" t="s">
         <v>39</v>
@@ -10234,25 +10231,25 @@
     </row>
     <row r="277" ht="15.75" customHeight="1">
       <c r="A277" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B277" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B277" s="1" t="s">
+      <c r="C277" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E277" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E277" s="1" t="s">
+      <c r="F277" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G277" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="F277" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G277" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>15</v>
@@ -10263,13 +10260,13 @@
     </row>
     <row r="278" ht="15.75" customHeight="1">
       <c r="A278" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>11</v>
@@ -10292,13 +10289,13 @@
     </row>
     <row r="279" ht="15.75" customHeight="1">
       <c r="A279" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>339</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>11</v>
@@ -10321,13 +10318,13 @@
     </row>
     <row r="280" ht="15.75" customHeight="1">
       <c r="A280" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B280" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B280" s="1" t="s">
-        <v>428</v>
-      </c>
       <c r="C280" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>11</v>
@@ -10350,13 +10347,13 @@
     </row>
     <row r="281" ht="15.75" customHeight="1">
       <c r="A281" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>11</v>
@@ -10379,13 +10376,13 @@
     </row>
     <row r="282" ht="15.75" customHeight="1">
       <c r="A282" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>11</v>
@@ -10408,13 +10405,13 @@
     </row>
     <row r="283" ht="15.75" customHeight="1">
       <c r="A283" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D283" s="1" t="s">
         <v>11</v>
@@ -10437,13 +10434,13 @@
     </row>
     <row r="284" ht="15.75" customHeight="1">
       <c r="A284" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D284" s="1" t="s">
         <v>11</v>
@@ -10466,19 +10463,19 @@
     </row>
     <row r="285" ht="15.75" customHeight="1">
       <c r="A285" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F285" s="5" t="s">
         <v>13</v>
@@ -10495,13 +10492,13 @@
     </row>
     <row r="286" ht="15.75" customHeight="1">
       <c r="A286" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D286" s="1" t="s">
         <v>11</v>
@@ -10524,19 +10521,19 @@
     </row>
     <row r="287" ht="15.75" customHeight="1">
       <c r="A287" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F287" s="5" t="s">
         <v>13</v>
@@ -10553,13 +10550,13 @@
     </row>
     <row r="288" ht="15.75" customHeight="1">
       <c r="A288" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>11</v>
@@ -10582,13 +10579,13 @@
     </row>
     <row r="289" ht="15.75" customHeight="1">
       <c r="A289" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D289" s="1" t="s">
         <v>11</v>
@@ -10611,13 +10608,13 @@
     </row>
     <row r="290" ht="15.75" customHeight="1">
       <c r="A290" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D290" s="1" t="s">
         <v>11</v>
@@ -10640,13 +10637,13 @@
     </row>
     <row r="291" ht="15.75" customHeight="1">
       <c r="A291" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D291" s="1" t="s">
         <v>11</v>
@@ -10669,13 +10666,13 @@
     </row>
     <row r="292" ht="15.75" customHeight="1">
       <c r="A292" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>11</v>
@@ -10698,13 +10695,13 @@
     </row>
     <row r="293" ht="15.75" customHeight="1">
       <c r="A293" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>11</v>
@@ -10727,13 +10724,13 @@
     </row>
     <row r="294" ht="15.75" customHeight="1">
       <c r="A294" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D294" s="1" t="s">
         <v>11</v>
@@ -10745,7 +10742,7 @@
         <v>13</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H294" s="1" t="s">
         <v>15</v>
@@ -10756,13 +10753,13 @@
     </row>
     <row r="295" ht="15.75" customHeight="1">
       <c r="A295" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B295" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B295" s="1" t="s">
-        <v>444</v>
-      </c>
       <c r="C295" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>11</v>
@@ -10785,25 +10782,25 @@
     </row>
     <row r="296" ht="15.75" customHeight="1">
       <c r="A296" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C296" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F296" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G296" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="D296" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F296" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G296" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="H296" s="1" t="s">
         <v>15</v>
@@ -10814,25 +10811,25 @@
     </row>
     <row r="297" ht="15.75" customHeight="1">
       <c r="A297" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B297" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F297" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G297" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D297" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F297" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G297" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>15</v>
@@ -10843,19 +10840,19 @@
     </row>
     <row r="298" ht="15.75" customHeight="1">
       <c r="A298" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E298" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D298" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="F298" s="5" t="s">
         <v>13</v>
@@ -10872,25 +10869,25 @@
     </row>
     <row r="299" ht="15.75" customHeight="1">
       <c r="A299" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E299" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G299" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="C299" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D299" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F299" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G299" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="H299" s="1" t="s">
         <v>15</v>
@@ -10901,19 +10898,19 @@
     </row>
     <row r="300" ht="15.75" customHeight="1">
       <c r="A300" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B300" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E300" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="C300" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="F300" s="2" t="s">
         <v>13</v>
@@ -10930,13 +10927,13 @@
     </row>
     <row r="301" ht="15.75" customHeight="1">
       <c r="A301" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B301" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B301" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="C301" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D301" s="1" t="s">
         <v>35</v>
@@ -10948,10 +10945,10 @@
         <v>20</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H301" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I301" s="1" t="s">
         <v>39</v>
@@ -10959,13 +10956,13 @@
     </row>
     <row r="302" ht="15.75" customHeight="1">
       <c r="A302" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>35</v>
@@ -10977,10 +10974,10 @@
         <v>20</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H302" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I302" s="1" t="s">
         <v>39</v>
@@ -10988,13 +10985,13 @@
     </row>
     <row r="303" ht="15.75" customHeight="1">
       <c r="A303" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>35</v>
@@ -11006,10 +11003,10 @@
         <v>20</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H303" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I303" s="1" t="s">
         <v>39</v>
@@ -11017,28 +11014,28 @@
     </row>
     <row r="304" ht="15.75" customHeight="1">
       <c r="A304" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F304" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H304" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I304" s="1" t="s">
         <v>39</v>
@@ -11046,13 +11043,13 @@
     </row>
     <row r="305" ht="15.75" customHeight="1">
       <c r="A305" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D305" s="1" t="s">
         <v>35</v>
@@ -11064,10 +11061,10 @@
         <v>20</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H305" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I305" s="1" t="s">
         <v>39</v>
@@ -11075,13 +11072,13 @@
     </row>
     <row r="306" ht="15.75" customHeight="1">
       <c r="A306" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B306" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B306" s="1" t="s">
-        <v>466</v>
-      </c>
       <c r="C306" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>35</v>
@@ -11093,10 +11090,10 @@
         <v>20</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H306" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I306" s="1" t="s">
         <v>39</v>
@@ -11104,13 +11101,13 @@
     </row>
     <row r="307" ht="15.75" customHeight="1">
       <c r="A307" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>35</v>
@@ -11122,10 +11119,10 @@
         <v>20</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H307" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I307" s="1" t="s">
         <v>39</v>
@@ -11133,25 +11130,25 @@
     </row>
     <row r="308" ht="15.75" customHeight="1">
       <c r="A308" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B308" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G308" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="C308" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E308" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F308" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G308" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>15</v>
@@ -11162,13 +11159,13 @@
     </row>
     <row r="309" ht="15.75" customHeight="1">
       <c r="A309" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D309" s="1" t="s">
         <v>11</v>
@@ -11180,7 +11177,7 @@
         <v>51</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H309" s="1" t="s">
         <v>15</v>
@@ -11191,13 +11188,13 @@
     </row>
     <row r="310" ht="15.75" customHeight="1">
       <c r="A310" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>347</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D310" s="1" t="s">
         <v>11</v>
@@ -11220,13 +11217,13 @@
     </row>
     <row r="311" ht="15.75" customHeight="1">
       <c r="A311" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B311" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B311" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="C311" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D311" s="1" t="s">
         <v>11</v>
@@ -11249,13 +11246,13 @@
     </row>
     <row r="312" ht="15.75" customHeight="1">
       <c r="A312" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D312" s="1" t="s">
         <v>11</v>
@@ -11267,7 +11264,7 @@
         <v>51</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>15</v>
@@ -11278,13 +11275,13 @@
     </row>
     <row r="313" ht="15.75" customHeight="1">
       <c r="A313" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>11</v>
@@ -11307,13 +11304,13 @@
     </row>
     <row r="314" ht="15.75" customHeight="1">
       <c r="A314" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D314" s="1" t="s">
         <v>35</v>
@@ -11325,10 +11322,10 @@
         <v>13</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H314" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I314" s="1" t="s">
         <v>39</v>
@@ -11336,13 +11333,13 @@
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D315" s="1" t="s">
         <v>11</v>
@@ -11354,7 +11351,7 @@
         <v>51</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>15</v>
@@ -11365,13 +11362,13 @@
     </row>
     <row r="316" ht="15.75" customHeight="1">
       <c r="A316" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D316" s="1" t="s">
         <v>35</v>
@@ -11383,10 +11380,10 @@
         <v>13</v>
       </c>
       <c r="G316" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H316" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I316" s="1" t="s">
         <v>39</v>
@@ -11394,25 +11391,25 @@
     </row>
     <row r="317" ht="15.75" customHeight="1">
       <c r="A317" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B317" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E317" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="C317" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="D317" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>485</v>
       </c>
       <c r="F317" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H317" s="1" t="s">
         <v>15</v>
@@ -11441,7 +11438,7 @@
         <v>51</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>15</v>
@@ -12021,7 +12018,7 @@
         <v>51</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H338" s="1" t="s">
         <v>15</v>
@@ -12035,7 +12032,7 @@
         <v>104</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>104</v>
@@ -12050,10 +12047,10 @@
         <v>20</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H339" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I339" s="1" t="s">
         <v>39</v>
@@ -12064,7 +12061,7 @@
         <v>104</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>104</v>
@@ -12079,10 +12076,10 @@
         <v>20</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H340" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I340" s="1" t="s">
         <v>39</v>
@@ -12093,7 +12090,7 @@
         <v>104</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>104</v>
@@ -12108,10 +12105,10 @@
         <v>13</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H341" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I341" s="1" t="s">
         <v>39</v>
@@ -12122,7 +12119,7 @@
         <v>104</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>104</v>
@@ -12137,10 +12134,10 @@
         <v>13</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H342" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I342" s="1" t="s">
         <v>39</v>
@@ -12151,7 +12148,7 @@
         <v>104</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>104</v>
@@ -12180,7 +12177,7 @@
         <v>104</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>104</v>
@@ -12209,7 +12206,7 @@
         <v>104</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>104</v>
@@ -12224,7 +12221,7 @@
         <v>13</v>
       </c>
       <c r="G345" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H345" s="1" t="s">
         <v>15</v>
@@ -12238,7 +12235,7 @@
         <v>104</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>104</v>
@@ -12253,7 +12250,7 @@
         <v>13</v>
       </c>
       <c r="G346" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H346" s="1" t="s">
         <v>15</v>
@@ -12267,7 +12264,7 @@
         <v>104</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>104</v>
@@ -12282,10 +12279,10 @@
         <v>13</v>
       </c>
       <c r="G347" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H347" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I347" s="1" t="s">
         <v>39</v>
@@ -12296,7 +12293,7 @@
         <v>104</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>104</v>
@@ -12311,10 +12308,10 @@
         <v>13</v>
       </c>
       <c r="G348" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H348" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I348" s="1" t="s">
         <v>39</v>
@@ -12325,7 +12322,7 @@
         <v>104</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>104</v>
@@ -12340,10 +12337,10 @@
         <v>20</v>
       </c>
       <c r="G349" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H349" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I349" s="1" t="s">
         <v>39</v>
@@ -12354,7 +12351,7 @@
         <v>104</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>104</v>
@@ -12369,10 +12366,10 @@
         <v>20</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H350" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I350" s="1" t="s">
         <v>39</v>
@@ -12383,7 +12380,7 @@
         <v>104</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>104</v>
@@ -12398,7 +12395,7 @@
         <v>13</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H351" s="1" t="s">
         <v>15</v>
@@ -12412,7 +12409,7 @@
         <v>104</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>104</v>
@@ -12427,7 +12424,7 @@
         <v>13</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H352" s="1" t="s">
         <v>15</v>
@@ -12441,7 +12438,7 @@
         <v>104</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>104</v>
@@ -12450,13 +12447,13 @@
         <v>11</v>
       </c>
       <c r="E353" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F353" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G353" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="F353" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G353" s="1" t="s">
-        <v>514</v>
       </c>
       <c r="H353" s="1" t="s">
         <v>15</v>
@@ -12470,7 +12467,7 @@
         <v>104</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>104</v>
@@ -12485,7 +12482,7 @@
         <v>13</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H354" s="1" t="s">
         <v>15</v>
@@ -12499,7 +12496,7 @@
         <v>104</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>104</v>
@@ -12514,7 +12511,7 @@
         <v>13</v>
       </c>
       <c r="G355" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H355" s="1" t="s">
         <v>15</v>
@@ -12528,7 +12525,7 @@
         <v>104</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>104</v>
@@ -12543,7 +12540,7 @@
         <v>51</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H356" s="1" t="s">
         <v>15</v>
@@ -12615,7 +12612,7 @@
         <v>104</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>104</v>
@@ -12630,7 +12627,7 @@
         <v>51</v>
       </c>
       <c r="G359" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H359" s="1" t="s">
         <v>15</v>
@@ -12641,13 +12638,13 @@
     </row>
     <row r="360" ht="15.75" customHeight="1">
       <c r="A360" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>11</v>
@@ -12670,7 +12667,7 @@
     </row>
     <row r="361" ht="15.75" customHeight="1">
       <c r="A361" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>30</v>
@@ -12699,13 +12696,13 @@
     </row>
     <row r="362" ht="15.75" customHeight="1">
       <c r="A362" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D362" s="1" t="s">
         <v>35</v>
@@ -12717,10 +12714,10 @@
         <v>13</v>
       </c>
       <c r="G362" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H362" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I362" s="1" t="s">
         <v>39</v>
@@ -12728,7 +12725,7 @@
     </row>
     <row r="363" ht="15.75" customHeight="1">
       <c r="A363" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>34</v>
@@ -12757,13 +12754,13 @@
     </row>
     <row r="364" ht="15.75" customHeight="1">
       <c r="A364" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D364" s="1" t="s">
         <v>11</v>
@@ -12786,7 +12783,7 @@
     </row>
     <row r="365" ht="15.75" customHeight="1">
       <c r="A365" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>32</v>
@@ -12815,13 +12812,13 @@
     </row>
     <row r="366" ht="15.75" customHeight="1">
       <c r="A366" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D366" s="1" t="s">
         <v>11</v>
@@ -12844,7 +12841,7 @@
     </row>
     <row r="367" ht="15.75" customHeight="1">
       <c r="A367" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>31</v>
@@ -12873,13 +12870,13 @@
     </row>
     <row r="368" ht="15.75" customHeight="1">
       <c r="A368" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D368" s="1" t="s">
         <v>35</v>
@@ -12891,10 +12888,10 @@
         <v>13</v>
       </c>
       <c r="G368" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H368" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I368" s="1" t="s">
         <v>39</v>
@@ -12902,7 +12899,7 @@
     </row>
     <row r="369" ht="15.75" customHeight="1">
       <c r="A369" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>40</v>

</xml_diff>